<commit_message>
Run some more tests
</commit_message>
<xml_diff>
--- a/R/Documentations des tests.xlsx
+++ b/R/Documentations des tests.xlsx
@@ -8,17 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uttroyes-my.sharepoint.com/personal/antonin_mathubert_utt_fr/Documents/Alécol/AlecolLearning/R/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="351" documentId="8_{20A9A9C9-FB76-46B1-B574-9B2B65F7BD0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{28E17577-E23B-47C9-B7D5-1608BF97A128}"/>
+  <xr:revisionPtr revIDLastSave="508" documentId="8_{20A9A9C9-FB76-46B1-B574-9B2B65F7BD0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{50FC3685-02BE-4097-B2F9-4898BF001891}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{ED9E0AB6-D481-4A8E-B548-322C4A50F4BD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="3" xr2:uid="{ED9E0AB6-D481-4A8E-B548-322C4A50F4BD}"/>
   </bookViews>
   <sheets>
     <sheet name="C01" sheetId="3" r:id="rId1"/>
-    <sheet name="S01" sheetId="8" r:id="rId2"/>
-    <sheet name="S02" sheetId="9" r:id="rId3"/>
-    <sheet name="T001" sheetId="1" r:id="rId4"/>
-    <sheet name="T002" sheetId="5" r:id="rId5"/>
-    <sheet name="T003" sheetId="10" r:id="rId6"/>
+    <sheet name="S03" sheetId="11" r:id="rId2"/>
+    <sheet name="T004" sheetId="12" r:id="rId3"/>
+    <sheet name="S01" sheetId="8" r:id="rId4"/>
+    <sheet name="T001" sheetId="1" r:id="rId5"/>
+    <sheet name="T002" sheetId="5" r:id="rId6"/>
+    <sheet name="T003" sheetId="10" r:id="rId7"/>
+    <sheet name="S02" sheetId="9" r:id="rId8"/>
+    <sheet name="T005" sheetId="13" r:id="rId9"/>
+    <sheet name="T006" sheetId="14" r:id="rId10"/>
+    <sheet name="T007" sheetId="15" r:id="rId11"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="49">
   <si>
     <t>ID de la campagne</t>
   </si>
@@ -77,9 +82,6 @@
     <t>ID du scénario</t>
   </si>
   <si>
-    <t>Trouver le jeu de questions le plus adapté pour analyser les résultats du test de mythologie</t>
-  </si>
-  <si>
     <t>Récap des tests du scénario</t>
   </si>
   <si>
@@ -138,13 +140,64 @@
   </si>
   <si>
     <t>A déterminer</t>
+  </si>
+  <si>
+    <t>Filtrer le jeu de questions avec comme indicateur le taux de bonnes réponses.</t>
+  </si>
+  <si>
+    <t>S03</t>
+  </si>
+  <si>
+    <t>T004</t>
+  </si>
+  <si>
+    <t>Retirer les questions qui apportent très peu d'information sur le score final obtenu améliore la qualité du test</t>
+  </si>
+  <si>
+    <t>C01/S03/T004</t>
+  </si>
+  <si>
+    <t>Améliorer le jeu de questions le plus adapté en se basant sur le point bisérial de corrélation dans le modèle à un paramètre</t>
+  </si>
+  <si>
+    <t>HYPOTHESE INVALIDEE</t>
+  </si>
+  <si>
+    <t>T006</t>
+  </si>
+  <si>
+    <t>Le modèle à deux paramètres apportent des résultats plus précis que le modèle de Rasch</t>
+  </si>
+  <si>
+    <t>C01/S02/T006</t>
+  </si>
+  <si>
+    <t>Le modèle à trois paramètres apportent des résultats plus précis que le modèle de Rasch</t>
+  </si>
+  <si>
+    <t>T005</t>
+  </si>
+  <si>
+    <t>C01/S02/T005</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> A déterminer</t>
+  </si>
+  <si>
+    <t>T007</t>
+  </si>
+  <si>
+    <t>C01/S02/T007</t>
+  </si>
+  <si>
+    <t>Le modèle à quatre paramètres apportent des résultats plus précis que le modèle de Rasch</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -232,8 +285,29 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="2" tint="-0.89999084444715716"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="2" tint="-0.749992370372631"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="11">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -293,8 +367,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -326,12 +412,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -375,90 +470,504 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Accent3" xfId="1" builtinId="37"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
+  <dxfs count="58">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
     </dxf>
@@ -794,32 +1303,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11EEA6E8-51A7-4B00-8ADF-352BD068DB5D}">
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="45" style="14" customWidth="1"/>
     <col min="2" max="2" width="4.85546875" style="15" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="33.7109375" style="21" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.7109375" style="20" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20.140625" style="15" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="33.7109375" style="21" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="33.7109375" style="20" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="0" style="16" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="33.7109375" style="23" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="33.7109375" style="22" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="5" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="C1" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="18" t="s">
+      <c r="E1" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="18" t="s">
+      <c r="G1" s="17" t="s">
         <v>6</v>
       </c>
     </row>
@@ -830,10 +1339,15 @@
       <c r="C2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="22" t="s">
+      <c r="E2" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="4"/>
+      <c r="F2" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" s="51" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="3" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="11"/>
@@ -849,65 +1363,95 @@
         <v>4</v>
       </c>
       <c r="B4" s="7"/>
-      <c r="C4" s="19" t="s">
+      <c r="C4" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="19"/>
-      <c r="G4" s="19"/>
+      <c r="E4" s="18"/>
+      <c r="G4" s="18"/>
     </row>
     <row r="5" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="13"/>
       <c r="B5" s="9"/>
-      <c r="C5" s="20"/>
+      <c r="C5" s="19"/>
       <c r="D5" s="9"/>
-      <c r="E5" s="20"/>
+      <c r="E5" s="19"/>
       <c r="F5"/>
       <c r="G5" s="1"/>
     </row>
     <row r="6" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="17" t="s">
+      <c r="A6" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="17"/>
-      <c r="C6" s="17"/>
-      <c r="D6" s="17"/>
-      <c r="E6" s="17"/>
-      <c r="F6" s="17"/>
-      <c r="G6" s="17"/>
+      <c r="B6" s="30"/>
+      <c r="C6" s="30"/>
+      <c r="D6" s="30"/>
+      <c r="E6" s="30"/>
+      <c r="F6" s="30"/>
+      <c r="G6" s="30"/>
     </row>
     <row r="7" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="str">
         <f>'S01'!A2</f>
         <v>S01</v>
       </c>
-      <c r="C7" s="21" t="str">
+      <c r="C7" s="20" t="str">
         <f>'S01'!C2</f>
-        <v>Trouver le jeu de questions le plus adapté pour analyser les résultats du test de mythologie</v>
-      </c>
-      <c r="E7" s="29" t="str">
+        <v>Filtrer le jeu de questions avec comme indicateur le taux de bonnes réponses.</v>
+      </c>
+      <c r="E7" s="27" t="str">
         <f>'S01'!E2</f>
         <v>Terminé !</v>
       </c>
-      <c r="G7" s="23" t="str">
+      <c r="G7" s="22" t="str">
         <f>'S01'!G$2</f>
         <v>Le jeu de question adapté se trouve dans le fichier "qcm_2_5_6_7_11_12_13_14_15_16_17_20_22_23_24.csv"</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="str">
-        <f>'S02'!A2</f>
+        <f>'S02'!$A$2</f>
         <v>S02</v>
       </c>
-      <c r="C8" s="21" t="str">
-        <f>'S02'!C2</f>
+      <c r="C8" s="20" t="str">
+        <f>'S02'!$C$2</f>
         <v>Trouver le modèle le plus adapté pour analyser le test de mythologie</v>
       </c>
-      <c r="E8" s="24" t="str">
-        <f>'S02'!E2</f>
+      <c r="E8" s="34" t="str">
+        <f>'S02'!$E$2</f>
         <v>En cours</v>
       </c>
-      <c r="G8" s="23" t="str">
-        <f>'S02'!G$2</f>
+      <c r="G8" s="22" t="str">
+        <f>'S02'!$G$2</f>
+        <v>A déterminer</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A9" s="14" t="str">
+        <f>'S03'!A2</f>
+        <v>S03</v>
+      </c>
+      <c r="B9" s="14">
+        <f>'S03'!B2</f>
+        <v>0</v>
+      </c>
+      <c r="C9" s="20" t="str">
+        <f>'S03'!C2</f>
+        <v>Améliorer le jeu de questions le plus adapté en se basant sur le point bisérial de corrélation dans le modèle à un paramètre</v>
+      </c>
+      <c r="D9" s="33">
+        <f>'S03'!D2</f>
+        <v>0</v>
+      </c>
+      <c r="E9" s="35" t="str">
+        <f>'S03'!E2</f>
+        <v>En cours</v>
+      </c>
+      <c r="F9" s="33">
+        <f>'S03'!F2</f>
+        <v>0</v>
+      </c>
+      <c r="G9" s="33" t="str">
+        <f>'S03'!G2</f>
         <v>A déterminer</v>
       </c>
     </row>
@@ -916,11 +1460,11 @@
   <mergeCells count="1">
     <mergeCell ref="A6:G6"/>
   </mergeCells>
-  <conditionalFormatting sqref="E2">
-    <cfRule type="containsText" dxfId="6" priority="2" operator="containsText" text="A faire">
+  <conditionalFormatting sqref="E2:G2">
+    <cfRule type="containsText" dxfId="57" priority="2" operator="containsText" text="A faire">
       <formula>NOT(ISERROR(SEARCH("A faire",E2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="5" priority="1" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="56" priority="1" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",E2)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -929,266 +1473,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2D2E0E1-A62E-42EC-B521-49A07A4C3AC1}">
-  <dimension ref="A1:G14"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="45" style="14" customWidth="1"/>
-    <col min="2" max="2" width="4.85546875" style="15" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="33.7109375" style="21" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.140625" style="15" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="33.7109375" style="21" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="0" style="16" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="33.7109375" style="23" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" s="5" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C1" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="E1" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="G1" s="18" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" s="6" customFormat="1" ht="78" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2" s="25" t="s">
-        <v>25</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="11"/>
-      <c r="B3"/>
-      <c r="C3" s="1"/>
-      <c r="D3"/>
-      <c r="E3" s="1"/>
-      <c r="F3"/>
-      <c r="G3" s="1"/>
-    </row>
-    <row r="4" spans="1:7" s="8" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="7"/>
-      <c r="C4" s="19" t="s">
-        <v>5</v>
-      </c>
-      <c r="E4" s="19"/>
-      <c r="G4" s="19"/>
-    </row>
-    <row r="5" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="13"/>
-      <c r="B5" s="9"/>
-      <c r="C5" s="20"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="20"/>
-      <c r="F5"/>
-      <c r="G5" s="1"/>
-    </row>
-    <row r="6" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" s="17"/>
-      <c r="C6" s="17"/>
-      <c r="D6" s="17"/>
-      <c r="E6" s="17"/>
-      <c r="F6" s="17"/>
-      <c r="G6" s="17"/>
-    </row>
-    <row r="7" spans="1:7" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="14" t="str">
-        <f>'T001'!A$2</f>
-        <v>T001</v>
-      </c>
-      <c r="C7" s="21" t="str">
-        <f>'T001'!C$2</f>
-        <v>Retirer les questions avec un taux de bonnes réponses &gt; 90% améliore les résultats</v>
-      </c>
-      <c r="E7" s="29" t="str">
-        <f>'T001'!E$2</f>
-        <v>Terminé !</v>
-      </c>
-      <c r="G7" s="30" t="str">
-        <f>'T001'!G$2</f>
-        <v>HYPOTHESE VALIDEE</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" s="14" t="str">
-        <f>'T002'!A$2</f>
-        <v>T002</v>
-      </c>
-      <c r="C8" s="21" t="str">
-        <f>'T002'!C$2</f>
-        <v>Retirer les questions avec un taux de bonnes réponses &lt; 25% améliore les résultats</v>
-      </c>
-      <c r="E8" s="29" t="str">
-        <f>'T002'!E$2</f>
-        <v>Terminé !</v>
-      </c>
-      <c r="F8" s="31"/>
-      <c r="G8" s="30" t="str">
-        <f>'T002'!G$2</f>
-        <v>HYPOTHESE VALIDEE</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" s="14" t="str">
-        <f>'T003'!A$2</f>
-        <v>T003</v>
-      </c>
-      <c r="C9" s="21" t="str">
-        <f>'T003'!C$2</f>
-        <v>Appliquer les hypothèses de T001 et T002 améliore les résultats</v>
-      </c>
-      <c r="E9" s="29" t="str">
-        <f>'T003'!E$2</f>
-        <v>Terminé !</v>
-      </c>
-      <c r="F9" s="31"/>
-      <c r="G9" s="30" t="str">
-        <f>'T003'!G$2</f>
-        <v>HYPOTHESE VALIDEE</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A6:G6"/>
-  </mergeCells>
-  <conditionalFormatting sqref="E7">
-    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",E7)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95B0C3FC-4F9F-4B2A-9D3E-1053E91F27B7}">
-  <dimension ref="A1:G14"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="45" style="14" customWidth="1"/>
-    <col min="2" max="2" width="4.85546875" style="15" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="33.7109375" style="21" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.140625" style="15" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="33.7109375" style="21" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="0" style="16" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="33.7109375" style="23" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" s="5" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C1" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="E1" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="G1" s="18" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" s="6" customFormat="1" ht="78" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="E2" s="22" t="s">
-        <v>8</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="11"/>
-      <c r="B3"/>
-      <c r="C3" s="1"/>
-      <c r="D3"/>
-      <c r="E3" s="1"/>
-      <c r="F3"/>
-      <c r="G3" s="1"/>
-    </row>
-    <row r="4" spans="1:7" s="8" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="7"/>
-      <c r="C4" s="19" t="s">
-        <v>5</v>
-      </c>
-      <c r="E4" s="19"/>
-      <c r="G4" s="19"/>
-    </row>
-    <row r="5" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="13"/>
-      <c r="B5" s="9"/>
-      <c r="C5" s="20"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="20"/>
-      <c r="F5"/>
-      <c r="G5" s="1"/>
-    </row>
-    <row r="6" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" s="17"/>
-      <c r="C6" s="17"/>
-      <c r="D6" s="17"/>
-      <c r="E6" s="17"/>
-      <c r="F6" s="17"/>
-      <c r="G6" s="17"/>
-    </row>
-    <row r="7" spans="1:7" ht="45.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A6:G6"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D40815D0-3EAB-4BC1-8DA5-1D201311502A}">
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31D1A081-8232-494C-A50E-9FEA18C8FAB2}">
   <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1205,36 +1495,36 @@
   <sheetData>
     <row r="1" spans="1:8" s="5" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="E1" s="18" t="s">
+      <c r="E1" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="18" t="s">
+      <c r="G1" s="17" t="s">
         <v>6</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:8" s="3" customFormat="1" ht="78" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C2" s="26" t="s">
-        <v>19</v>
-      </c>
-      <c r="E2" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="E2" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="G2" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="G2" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="H2" s="28" t="s">
-        <v>23</v>
+      <c r="H2" s="26" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="21" hidden="1" x14ac:dyDescent="0.25">
@@ -1248,30 +1538,44 @@
         <v>4</v>
       </c>
       <c r="B4" s="7"/>
-      <c r="C4" s="19" t="s">
+      <c r="C4" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="19"/>
-      <c r="G4" s="19"/>
+      <c r="E4" s="18"/>
+      <c r="G4" s="18"/>
     </row>
     <row r="5" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
     <row r="14" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <conditionalFormatting sqref="E2">
-    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="35" priority="4" operator="containsText" text="Terminé !">
+      <formula>NOT(ISERROR(SEARCH("Terminé !",E2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="34" priority="5" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",E2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G2">
+    <cfRule type="containsText" dxfId="33" priority="1" operator="containsText" text="HYPOTHESE INVALIDEE">
+      <formula>NOT(ISERROR(SEARCH("HYPOTHESE INVALIDEE",G2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="32" priority="2" operator="containsText" text="HYPOTHESE VALIDEE">
+      <formula>NOT(ISERROR(SEARCH("HYPOTHESE VALIDEE",G2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="31" priority="3" operator="containsText" text="?">
+      <formula>NOT(ISERROR(SEARCH("?",G2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0D5380E-4249-47C3-BE24-ECF1E8746998}">
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94CD04C3-D03E-4FD8-AC30-0B375717B6EA}">
   <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A1:XFD1048576"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1288,36 +1592,36 @@
   <sheetData>
     <row r="1" spans="1:8" s="5" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="E1" s="18" t="s">
+      <c r="E1" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="18" t="s">
+      <c r="G1" s="17" t="s">
         <v>6</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:8" s="3" customFormat="1" ht="78" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C2" s="26" t="s">
-        <v>21</v>
-      </c>
-      <c r="E2" s="27" t="s">
-        <v>25</v>
-      </c>
-      <c r="G2" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="H2" s="28" t="s">
-        <v>24</v>
+        <v>46</v>
+      </c>
+      <c r="C2" s="24" t="s">
+        <v>48</v>
+      </c>
+      <c r="E2" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="H2" s="26" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="21" hidden="1" x14ac:dyDescent="0.25">
@@ -1331,30 +1635,171 @@
         <v>4</v>
       </c>
       <c r="B4" s="7"/>
-      <c r="C4" s="19" t="s">
+      <c r="C4" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="19"/>
-      <c r="G4" s="19"/>
+      <c r="E4" s="18"/>
+      <c r="G4" s="18"/>
     </row>
     <row r="5" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
     <row r="14" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <conditionalFormatting sqref="E2">
-    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="4" priority="4" operator="containsText" text="Terminé !">
+      <formula>NOT(ISERROR(SEARCH("Terminé !",E2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="3" priority="5" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",E2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G2">
+    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="HYPOTHESE INVALIDEE">
+      <formula>NOT(ISERROR(SEARCH("HYPOTHESE INVALIDEE",G2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="HYPOTHESE VALIDEE">
+      <formula>NOT(ISERROR(SEARCH("HYPOTHESE VALIDEE",G2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="?">
+      <formula>NOT(ISERROR(SEARCH("?",G2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{164A21DB-C16D-438E-BE34-612B29EFC02D}">
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5978198F-30DD-4488-8862-549D1E68CAF3}">
+  <dimension ref="A1:G14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="45" style="14" customWidth="1"/>
+    <col min="2" max="2" width="4.85546875" style="15" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="33.7109375" style="20" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.140625" style="15" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="33.7109375" style="20" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="0" style="16" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="33.7109375" style="22" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" s="5" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="17" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" s="6" customFormat="1" ht="78" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="E2" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="11"/>
+      <c r="B3"/>
+      <c r="C3" s="1"/>
+      <c r="D3"/>
+      <c r="E3" s="1"/>
+      <c r="F3"/>
+      <c r="G3" s="1"/>
+    </row>
+    <row r="4" spans="1:7" s="8" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="7"/>
+      <c r="C4" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="18"/>
+      <c r="G4" s="18"/>
+    </row>
+    <row r="5" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="13"/>
+      <c r="B5" s="9"/>
+      <c r="C5" s="19"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="19"/>
+      <c r="F5"/>
+      <c r="G5" s="1"/>
+    </row>
+    <row r="6" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="30" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="30"/>
+      <c r="C6" s="30"/>
+      <c r="D6" s="30"/>
+      <c r="E6" s="30"/>
+      <c r="F6" s="30"/>
+      <c r="G6" s="30"/>
+    </row>
+    <row r="7" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A7" s="14" t="str">
+        <f>'T004'!A2</f>
+        <v>T004</v>
+      </c>
+      <c r="B7" s="14">
+        <f>'T004'!B2</f>
+        <v>0</v>
+      </c>
+      <c r="C7" s="20" t="str">
+        <f>'T004'!C2</f>
+        <v>Retirer les questions qui apportent très peu d'information sur le score final obtenu améliore la qualité du test</v>
+      </c>
+      <c r="D7" s="14">
+        <f>'T004'!D2</f>
+        <v>0</v>
+      </c>
+      <c r="E7" s="37" t="str">
+        <f>'T004'!E2</f>
+        <v>Terminé !</v>
+      </c>
+      <c r="F7" s="14">
+        <f>'T004'!F2</f>
+        <v>0</v>
+      </c>
+      <c r="G7" s="38" t="str">
+        <f>'T004'!G2</f>
+        <v>HYPOTHESE INVALIDEE</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A6:G6"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{902EA4CC-00CD-4769-A9ED-64F8C80D5E46}">
   <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1371,36 +1816,36 @@
   <sheetData>
     <row r="1" spans="1:8" s="5" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="E1" s="18" t="s">
+      <c r="E1" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="18" t="s">
+      <c r="G1" s="17" t="s">
         <v>6</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:8" s="3" customFormat="1" ht="78" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C2" s="26" t="s">
-        <v>28</v>
-      </c>
-      <c r="E2" s="27" t="s">
-        <v>25</v>
-      </c>
-      <c r="G2" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="H2" s="28" t="s">
-        <v>29</v>
+        <v>34</v>
+      </c>
+      <c r="C2" s="31" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="G2" s="36" t="s">
+        <v>38</v>
+      </c>
+      <c r="H2" s="26" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="21" hidden="1" x14ac:dyDescent="0.25">
@@ -1414,18 +1859,759 @@
         <v>4</v>
       </c>
       <c r="B4" s="7"/>
-      <c r="C4" s="19" t="s">
+      <c r="C4" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="19"/>
-      <c r="G4" s="19"/>
+      <c r="E4" s="18"/>
+      <c r="G4" s="18"/>
     </row>
     <row r="5" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
     <row r="14" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <conditionalFormatting sqref="E2">
-    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="53" priority="3" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",E2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G2">
+    <cfRule type="containsText" dxfId="51" priority="1" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",G2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2D2E0E1-A62E-42EC-B521-49A07A4C3AC1}">
+  <dimension ref="A1:G14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="45" style="14" customWidth="1"/>
+    <col min="2" max="2" width="4.85546875" style="15" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="33.7109375" style="20" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.140625" style="15" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="33.7109375" style="20" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="0" style="16" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="33.7109375" style="22" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" s="5" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="17" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" s="6" customFormat="1" ht="78" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="11"/>
+      <c r="B3"/>
+      <c r="C3" s="1"/>
+      <c r="D3"/>
+      <c r="E3" s="1"/>
+      <c r="F3"/>
+      <c r="G3" s="1"/>
+    </row>
+    <row r="4" spans="1:7" s="8" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="7"/>
+      <c r="C4" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="18"/>
+      <c r="G4" s="18"/>
+    </row>
+    <row r="5" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="13"/>
+      <c r="B5" s="9"/>
+      <c r="C5" s="19"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="19"/>
+      <c r="F5"/>
+      <c r="G5" s="1"/>
+    </row>
+    <row r="6" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="30" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="30"/>
+      <c r="C6" s="30"/>
+      <c r="D6" s="30"/>
+      <c r="E6" s="30"/>
+      <c r="F6" s="30"/>
+      <c r="G6" s="30"/>
+    </row>
+    <row r="7" spans="1:7" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="14" t="str">
+        <f>'T001'!A$2</f>
+        <v>T001</v>
+      </c>
+      <c r="C7" s="20" t="str">
+        <f>'T001'!C$2</f>
+        <v>Retirer les questions avec un taux de bonnes réponses &gt; 90% améliore les résultats</v>
+      </c>
+      <c r="E7" s="27" t="str">
+        <f>'T001'!E$2</f>
+        <v>Terminé !</v>
+      </c>
+      <c r="G7" s="28" t="str">
+        <f>'T001'!G$2</f>
+        <v>HYPOTHESE VALIDEE</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A8" s="14" t="str">
+        <f>'T002'!A$2</f>
+        <v>T002</v>
+      </c>
+      <c r="C8" s="20" t="str">
+        <f>'T002'!C$2</f>
+        <v>Retirer les questions avec un taux de bonnes réponses &lt; 25% améliore les résultats</v>
+      </c>
+      <c r="E8" s="27" t="str">
+        <f>'T002'!E$2</f>
+        <v>Terminé !</v>
+      </c>
+      <c r="F8" s="29"/>
+      <c r="G8" s="28" t="str">
+        <f>'T002'!G$2</f>
+        <v>HYPOTHESE VALIDEE</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="14" t="str">
+        <f>'T003'!A$2</f>
+        <v>T003</v>
+      </c>
+      <c r="C9" s="20" t="str">
+        <f>'T003'!C$2</f>
+        <v>Appliquer les hypothèses de T001 et T002 améliore les résultats</v>
+      </c>
+      <c r="E9" s="27" t="str">
+        <f>'T003'!E$2</f>
+        <v>Terminé !</v>
+      </c>
+      <c r="F9" s="29"/>
+      <c r="G9" s="28" t="str">
+        <f>'T003'!G$2</f>
+        <v>HYPOTHESE VALIDEE</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A6:G6"/>
+  </mergeCells>
+  <conditionalFormatting sqref="E7">
+    <cfRule type="containsText" dxfId="30" priority="3" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",E7)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E1:E1048576">
+    <cfRule type="containsText" dxfId="29" priority="2" operator="containsText" text="Terminé !">
+      <formula>NOT(ISERROR(SEARCH("Terminé !",E1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="28" priority="1" operator="containsText" text="Annulé">
+      <formula>NOT(ISERROR(SEARCH("Annulé",E1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D40815D0-3EAB-4BC1-8DA5-1D201311502A}">
+  <dimension ref="A1:H14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G2" sqref="E2:G2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="45" customWidth="1"/>
+    <col min="2" max="2" width="4.85546875" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="33.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.140625" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="33.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="0" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="33.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" s="5" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" s="3" customFormat="1" ht="78" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="G2" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="H2" s="26" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="21" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="11"/>
+      <c r="C3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="G3" s="1"/>
+    </row>
+    <row r="4" spans="1:8" s="8" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="7"/>
+      <c r="C4" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="18"/>
+      <c r="G4" s="18"/>
+    </row>
+    <row r="5" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <conditionalFormatting sqref="E2">
+    <cfRule type="containsText" dxfId="47" priority="5" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",E2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="46" priority="4" operator="containsText" text="Terminé !">
+      <formula>NOT(ISERROR(SEARCH("Terminé !",E2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G2">
+    <cfRule type="containsText" dxfId="44" priority="3" operator="containsText" text="?">
+      <formula>NOT(ISERROR(SEARCH("?",G2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="45" priority="2" operator="containsText" text="HYPOTHESE VALIDEE">
+      <formula>NOT(ISERROR(SEARCH("HYPOTHESE VALIDEE",G2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="43" priority="1" operator="containsText" text="HYPOTHESE INVALIDEE">
+      <formula>NOT(ISERROR(SEARCH("HYPOTHESE INVALIDEE",G2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0D5380E-4249-47C3-BE24-ECF1E8746998}">
+  <dimension ref="A1:H14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="45" customWidth="1"/>
+    <col min="2" max="2" width="4.85546875" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="33.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.140625" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="33.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="0" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="33.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" s="5" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" s="3" customFormat="1" ht="78" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="G2" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="H2" s="26" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="21" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="11"/>
+      <c r="C3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="G3" s="1"/>
+    </row>
+    <row r="4" spans="1:8" s="8" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="7"/>
+      <c r="C4" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="18"/>
+      <c r="G4" s="18"/>
+    </row>
+    <row r="5" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <conditionalFormatting sqref="E2">
+    <cfRule type="containsText" dxfId="55" priority="1" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",E2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{164A21DB-C16D-438E-BE34-612B29EFC02D}">
+  <dimension ref="A1:H14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="45" customWidth="1"/>
+    <col min="2" max="2" width="4.85546875" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="33.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.140625" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="33.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="0" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="33.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" s="5" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" s="3" customFormat="1" ht="78" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="E2" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="G2" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="H2" s="26" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="21" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="11"/>
+      <c r="C3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="G3" s="1"/>
+    </row>
+    <row r="4" spans="1:8" s="8" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="7"/>
+      <c r="C4" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="18"/>
+      <c r="G4" s="18"/>
+    </row>
+    <row r="5" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <conditionalFormatting sqref="E2">
+    <cfRule type="containsText" dxfId="54" priority="1" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",E2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95B0C3FC-4F9F-4B2A-9D3E-1053E91F27B7}">
+  <dimension ref="A1:G14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="45" style="14" customWidth="1"/>
+    <col min="2" max="2" width="4.85546875" style="15" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="33.7109375" style="20" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.140625" style="15" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="33.7109375" style="39" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="0" style="16" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="33.7109375" style="45" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" s="5" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="17" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" s="6" customFormat="1" ht="78" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="46" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="47"/>
+      <c r="C2" s="48" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" s="47"/>
+      <c r="E2" s="49" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="47"/>
+      <c r="G2" s="50" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="11"/>
+      <c r="B3"/>
+      <c r="C3" s="43"/>
+      <c r="D3"/>
+      <c r="E3" s="40"/>
+      <c r="F3"/>
+      <c r="G3" s="40"/>
+    </row>
+    <row r="4" spans="1:7" s="8" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="7"/>
+      <c r="C4" s="44" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="41"/>
+      <c r="G4" s="41"/>
+    </row>
+    <row r="5" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="13"/>
+      <c r="B5" s="9"/>
+      <c r="C5" s="19"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="42"/>
+      <c r="F5"/>
+      <c r="G5" s="40"/>
+    </row>
+    <row r="6" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="30" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="30"/>
+      <c r="C6" s="30"/>
+      <c r="D6" s="30"/>
+      <c r="E6" s="30"/>
+      <c r="F6" s="30"/>
+      <c r="G6" s="30"/>
+    </row>
+    <row r="7" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="14" t="str">
+        <f>'T005'!A2</f>
+        <v>T005</v>
+      </c>
+      <c r="B7" s="14">
+        <f>'T005'!B2</f>
+        <v>0</v>
+      </c>
+      <c r="C7" s="20" t="str">
+        <f>'T005'!C2</f>
+        <v>Le modèle à deux paramètres apportent des résultats plus précis que le modèle de Rasch</v>
+      </c>
+      <c r="D7" s="20">
+        <f>'T005'!D2</f>
+        <v>0</v>
+      </c>
+      <c r="E7" s="39" t="str">
+        <f>'T005'!E2</f>
+        <v>Terminé !</v>
+      </c>
+      <c r="F7" s="14">
+        <f>'T005'!F2</f>
+        <v>0</v>
+      </c>
+      <c r="G7" s="32" t="str">
+        <f>'T005'!G2</f>
+        <v>HYPOTHESE VALIDEE</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A8" s="14" t="str">
+        <f>'T006'!A2</f>
+        <v>T006</v>
+      </c>
+      <c r="B8" s="14">
+        <f>'T006'!B2</f>
+        <v>0</v>
+      </c>
+      <c r="C8" s="20" t="str">
+        <f>'T006'!C2</f>
+        <v>Le modèle à trois paramètres apportent des résultats plus précis que le modèle de Rasch</v>
+      </c>
+      <c r="D8" s="20">
+        <f>'T006'!D2</f>
+        <v>0</v>
+      </c>
+      <c r="E8" s="39" t="str">
+        <f>'T006'!E2</f>
+        <v>Terminé !</v>
+      </c>
+      <c r="F8" s="14">
+        <f>'T006'!F2</f>
+        <v>0</v>
+      </c>
+      <c r="G8" s="32" t="str">
+        <f>'T006'!G2</f>
+        <v>HYPOTHESE VALIDEE</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="14" t="str">
+        <f>'T007'!A2</f>
+        <v>T007</v>
+      </c>
+      <c r="B9" s="14">
+        <f>'T007'!B2</f>
+        <v>0</v>
+      </c>
+      <c r="C9" s="20" t="str">
+        <f>'T007'!C2</f>
+        <v>Le modèle à quatre paramètres apportent des résultats plus précis que le modèle de Rasch</v>
+      </c>
+      <c r="D9" s="14">
+        <f>'T007'!D2</f>
+        <v>0</v>
+      </c>
+      <c r="E9" s="32" t="str">
+        <f>'T007'!E2</f>
+        <v>En cours</v>
+      </c>
+      <c r="F9" s="14">
+        <f>'T007'!F2</f>
+        <v>0</v>
+      </c>
+      <c r="G9" s="32" t="str">
+        <f>'T007'!G2</f>
+        <v xml:space="preserve"> A déterminer</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A6:G6"/>
+  </mergeCells>
+  <conditionalFormatting sqref="A1:G1048576">
+    <cfRule type="containsText" dxfId="10" priority="5" operator="containsText" text="Annulé">
+      <formula>NOT(ISERROR(SEARCH("Annulé",A1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="9" priority="6" operator="containsText" text="Terminé !">
+      <formula>NOT(ISERROR(SEARCH("Terminé !",A1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="8" priority="4" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",A1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G1:G1048576">
+    <cfRule type="containsText" dxfId="6" priority="3" operator="containsText" text="A déterminer">
+      <formula>NOT(ISERROR(SEARCH("A déterminer",G1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="7" priority="2" operator="containsText" text="HYPOTHESE VALIDEE">
+      <formula>NOT(ISERROR(SEARCH("HYPOTHESE VALIDEE",G1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="5" priority="1" operator="containsText" text="HYPOTHESE INVALIDEE">
+      <formula>NOT(ISERROR(SEARCH("HYPOTHESE INVALIDEE",G1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4104569-12CE-436F-A40A-94DD5A149B50}">
+  <dimension ref="A1:H14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="45" customWidth="1"/>
+    <col min="2" max="2" width="4.85546875" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="33.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.140625" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="33.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="0" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="33.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" s="5" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" s="3" customFormat="1" ht="78" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="E2" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="G2" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="H2" s="26" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="21" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="11"/>
+      <c r="C3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="G3" s="1"/>
+    </row>
+    <row r="4" spans="1:8" s="8" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="7"/>
+      <c r="C4" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="18"/>
+      <c r="G4" s="18"/>
+    </row>
+    <row r="5" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <conditionalFormatting sqref="E2">
+    <cfRule type="containsText" dxfId="39" priority="4" operator="containsText" text="Terminé !">
+      <formula>NOT(ISERROR(SEARCH("Terminé !",E2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="40" priority="5" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",E2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G2">
+    <cfRule type="containsText" dxfId="36" priority="1" operator="containsText" text="HYPOTHESE INVALIDEE">
+      <formula>NOT(ISERROR(SEARCH("HYPOTHESE INVALIDEE",G2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="37" priority="2" operator="containsText" text="HYPOTHESE VALIDEE">
+      <formula>NOT(ISERROR(SEARCH("HYPOTHESE VALIDEE",G2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="38" priority="3" operator="containsText" text="?">
+      <formula>NOT(ISERROR(SEARCH("?",G2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>